<commit_message>
docs: Documentação atualizada com o novo processo de carga dos dados.
</commit_message>
<xml_diff>
--- a/src/data/database.xlsx
+++ b/src/data/database.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,11 @@
           <t>resultado</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -458,32 +463,66 @@
         <v>5000</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="D2" t="n">
         <v>1000</v>
       </c>
       <c r="E2" t="n">
-        <v>5500</v>
+        <v>2000</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-05-13 22:02:38</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Maria</t>
+          <t>Claudia</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5231</v>
+        <v>1900</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D3" t="n">
         <v>1000</v>
       </c>
       <c r="E3" t="n">
-        <v>2046.2</v>
+        <v>1950</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-05-13 22:02:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Gabrielle</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1750</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-05-13 22:03:00</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>